<commit_message>
Update 602 - Eng Cases Reported by specimen date.xlsx
</commit_message>
<xml_diff>
--- a/602 - Eng Cases Reported by specimen date.xlsx
+++ b/602 - Eng Cases Reported by specimen date.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\hp-server\ServerFolders\Documents\Covid-19\Covid data\_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB59513A-48AD-4C49-8CC0-C972A8940117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC065F1-443D-4C89-AF6B-B53BF1C3F284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="60" windowWidth="21630" windowHeight="20910" activeTab="2" xr2:uid="{4FC3F2A8-793A-4932-B6D9-8372FE28C2B0}"/>
   </bookViews>
@@ -647,6 +647,12 @@
       <numFmt numFmtId="164" formatCode="d\ mmm\ yy"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="165" formatCode="d/m/yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
@@ -666,12 +672,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="d/m/yy;@"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -6173,7 +6173,7 @@
         <c:axId val="1003354336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="100000"/>
+          <c:max val="30000"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -6234,7 +6234,7 @@
         <c:crossAx val="1003356632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:minorUnit val="10000"/>
+        <c:minorUnit val="5000"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -16781,7 +16781,7 @@
         <c:axId val="1003354336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="20000"/>
+          <c:max val="15000"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -18732,10 +18732,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DB4F2183-A76F-4F57-AC0B-113838B0C44D}" name="daily_PHE_update" displayName="daily_PHE_update" ref="A1:G861" tableType="queryTable" totalsRowCount="1">
   <autoFilter ref="A1:G860" xr:uid="{6792228A-E583-499A-AA0E-E9D8D3B668FE}"/>
   <tableColumns count="7">
-    <tableColumn id="3" xr3:uid="{36B9E94A-7B32-4C4D-94DE-4023263F8521}" uniqueName="3" name="areaCode" queryTableFieldId="3" dataDxfId="4" totalsRowDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{537AAC26-7168-4F65-99DE-41DDBEC2C33E}" uniqueName="4" name="areaName" queryTableFieldId="4" dataDxfId="3" totalsRowDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{22E5A6E2-BDF0-479D-994F-93EA6C449FC1}" uniqueName="2" name="areaType" queryTableFieldId="2" dataDxfId="2" totalsRowDxfId="7"/>
-    <tableColumn id="1" xr3:uid="{9E40D7E8-496A-4CFD-B4BF-AEF250D34948}" uniqueName="1" name="date" queryTableFieldId="1" dataDxfId="1" totalsRowDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{36B9E94A-7B32-4C4D-94DE-4023263F8521}" uniqueName="3" name="areaCode" queryTableFieldId="3" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{537AAC26-7168-4F65-99DE-41DDBEC2C33E}" uniqueName="4" name="areaName" queryTableFieldId="4" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{22E5A6E2-BDF0-479D-994F-93EA6C449FC1}" uniqueName="2" name="areaType" queryTableFieldId="2" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{9E40D7E8-496A-4CFD-B4BF-AEF250D34948}" uniqueName="1" name="date" queryTableFieldId="1" dataDxfId="3" totalsRowDxfId="2"/>
     <tableColumn id="7" xr3:uid="{CF6E145E-EEE4-43EA-B16E-01BCC6C7208E}" uniqueName="7" name="changeInNewCasesBySpecimenDate" totalsRowFunction="custom" queryTableFieldId="7">
       <totalsRowFormula>SUM(E2:E860)</totalsRowFormula>
     </tableColumn>
@@ -18747,7 +18747,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4CDD3B96-61A9-46BB-AC47-E84AC61F093A}" name="Table10" displayName="Table10" ref="A1:EG25" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4CDD3B96-61A9-46BB-AC47-E84AC61F093A}" name="Table10" displayName="Table10" ref="A1:EG25" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:EG25" xr:uid="{4CDD3B96-61A9-46BB-AC47-E84AC61F093A}"/>
   <tableColumns count="137">
     <tableColumn id="1" xr3:uid="{CF0493B3-D1A8-45D2-9B7B-CC8C86E7F345}" name="Column1"/>
@@ -44989,7 +44989,7 @@
         <v>185</v>
       </c>
       <c r="EI22">
-        <f t="shared" ref="EG22:EI22" si="0">SUM((EI2-EI20)-SUM(EI3:EI10))</f>
+        <f t="shared" ref="EI22" si="0">SUM((EI2-EI20)-SUM(EI3:EI10))</f>
         <v>185</v>
       </c>
     </row>
@@ -45321,7 +45321,7 @@
   <dimension ref="A1:U43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="AZ40" sqref="AZ40"/>
+      <selection activeCell="BB56" sqref="BB56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>